<commit_message>
cohort six email addresses
</commit_message>
<xml_diff>
--- a/cohort_Emails.xlsx
+++ b/cohort_Emails.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -44,10 +44,190 @@
     <t>linetnalubega1@gmail.com</t>
   </si>
   <si>
-    <t>Shainah Hadley</t>
-  </si>
-  <si>
     <t>shainahmay@gmail.com</t>
+  </si>
+  <si>
+    <t>Pauline Nalwanga</t>
+  </si>
+  <si>
+    <t>paulinon141@gmail.com</t>
+  </si>
+  <si>
+    <t>Ismail Asega</t>
+  </si>
+  <si>
+    <t>asega03@gmail.com</t>
+  </si>
+  <si>
+    <t>Hadley Shainah</t>
+  </si>
+  <si>
+    <t>Conrad Waako</t>
+  </si>
+  <si>
+    <t>Eliezerconrad256@gmail.com</t>
+  </si>
+  <si>
+    <t>Mercy Wamanga</t>
+  </si>
+  <si>
+    <t>tashma191@gmail.com</t>
+  </si>
+  <si>
+    <t>Yusuf Nviiri</t>
+  </si>
+  <si>
+    <t>yusufnviiri@gmail.com</t>
+  </si>
+  <si>
+    <t>Derrick Ainembabazi</t>
+  </si>
+  <si>
+    <t>ainederrick23@gmail.com</t>
+  </si>
+  <si>
+    <t>Zainab Adu</t>
+  </si>
+  <si>
+    <t>moniqueadu3@gmail.com</t>
+  </si>
+  <si>
+    <t>Joanita Nsimbe</t>
+  </si>
+  <si>
+    <t>joanita.nsimbe@gmail.com</t>
+  </si>
+  <si>
+    <t>Sarah Olila</t>
+  </si>
+  <si>
+    <t>olila.sarah70@gmail.com</t>
+  </si>
+  <si>
+    <t>Ephrance Kisakye</t>
+  </si>
+  <si>
+    <t>nanfumaephrance@gmail.com</t>
+  </si>
+  <si>
+    <t>Liz Kamugisha</t>
+  </si>
+  <si>
+    <t>liz.kamugisha@gmail.com</t>
+  </si>
+  <si>
+    <t>Esau Kakuru</t>
+  </si>
+  <si>
+    <t>Esaukaks@gmail.com</t>
+  </si>
+  <si>
+    <t>Travor Kimbugwe</t>
+  </si>
+  <si>
+    <t>kimbugwetravor99@gmail.com</t>
+  </si>
+  <si>
+    <t>Sylvia Boonabana</t>
+  </si>
+  <si>
+    <t>sylviaboona2@gmail.com</t>
+  </si>
+  <si>
+    <t>Arthur Mukwaya</t>
+  </si>
+  <si>
+    <t>arthurmukwaya@gmail.com</t>
+  </si>
+  <si>
+    <t>Samuel Okwalinga</t>
+  </si>
+  <si>
+    <t>sam.tek727@gmail.com</t>
+  </si>
+  <si>
+    <t>Benjamin Otim</t>
+  </si>
+  <si>
+    <t>benjaminmunguriek@gmail.com</t>
+  </si>
+  <si>
+    <t>Rino Kitimbo</t>
+  </si>
+  <si>
+    <t>kitimborinoemma0580@gmail.com</t>
+  </si>
+  <si>
+    <t>Beatrice Akatukunda</t>
+  </si>
+  <si>
+    <t>beatrice.kunda96@gmail.com</t>
+  </si>
+  <si>
+    <t>Emmanuel Kodowo Mensah</t>
+  </si>
+  <si>
+    <t>emailkmensah@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sheena Tushabe </t>
+  </si>
+  <si>
+    <t>turyasheena@gmail.com</t>
+  </si>
+  <si>
+    <t>Mariat Ndagire</t>
+  </si>
+  <si>
+    <t>mariatndagire28@gmail.com</t>
+  </si>
+  <si>
+    <t>Matia Kaweesi</t>
+  </si>
+  <si>
+    <t>Matiakaweesi@gmail.com</t>
+  </si>
+  <si>
+    <t>Paul Livingstone</t>
+  </si>
+  <si>
+    <t>senopaul@gmail.com</t>
+  </si>
+  <si>
+    <t>Diana Apolat</t>
+  </si>
+  <si>
+    <t>apolatdiana@gmail.com</t>
+  </si>
+  <si>
+    <t>Nickson Kiwumulo</t>
+  </si>
+  <si>
+    <t>nicksonk2017@gmail.com</t>
+  </si>
+  <si>
+    <t>Theophile Sugira</t>
+  </si>
+  <si>
+    <t>nyembless@gmail.com</t>
+  </si>
+  <si>
+    <t>Kenneth Clein Ouma</t>
+  </si>
+  <si>
+    <t>kennethclein4@gmail.com</t>
+  </si>
+  <si>
+    <t>Immaculate Nakirya</t>
+  </si>
+  <si>
+    <t>immynakirya2@gmail.com</t>
+  </si>
+  <si>
+    <t>Patricia Nekesa</t>
+  </si>
+  <si>
+    <t>nekepatri@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -390,10 +570,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -412,33 +593,306 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>7</v>
       </c>
+      <c r="B25" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="A2:B34">
+    <sortCondition ref="A2"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B14" r:id="rId1"/>
+    <hyperlink ref="B17" r:id="rId2"/>
+    <hyperlink ref="B11" r:id="rId3"/>
+    <hyperlink ref="B25" r:id="rId4"/>
+    <hyperlink ref="B13" r:id="rId5"/>
+    <hyperlink ref="B5" r:id="rId6"/>
+    <hyperlink ref="B21" r:id="rId7"/>
+    <hyperlink ref="B33" r:id="rId8"/>
+    <hyperlink ref="B6" r:id="rId9"/>
+    <hyperlink ref="B34" r:id="rId10"/>
+    <hyperlink ref="B15" r:id="rId11"/>
+    <hyperlink ref="B28" r:id="rId12"/>
+    <hyperlink ref="B9" r:id="rId13"/>
+    <hyperlink ref="B18" r:id="rId14"/>
+    <hyperlink ref="B10" r:id="rId15"/>
+    <hyperlink ref="B32" r:id="rId16"/>
+    <hyperlink ref="B30" r:id="rId17"/>
+    <hyperlink ref="B2" r:id="rId18"/>
+    <hyperlink ref="B27" r:id="rId19"/>
+    <hyperlink ref="B4" r:id="rId20"/>
+    <hyperlink ref="B26" r:id="rId21"/>
+    <hyperlink ref="B3" r:id="rId22"/>
+    <hyperlink ref="B8" r:id="rId23"/>
+    <hyperlink ref="B29" r:id="rId24"/>
+    <hyperlink ref="B19" r:id="rId25"/>
+    <hyperlink ref="B20" r:id="rId26"/>
+    <hyperlink ref="B24" r:id="rId27"/>
+    <hyperlink ref="B7" r:id="rId28"/>
+    <hyperlink ref="B22" r:id="rId29"/>
+    <hyperlink ref="B31" r:id="rId30"/>
+    <hyperlink ref="B16" r:id="rId31"/>
+    <hyperlink ref="B12" r:id="rId32"/>
+    <hyperlink ref="B23" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added tesi and martin anderson emails
</commit_message>
<xml_diff>
--- a/cohort_Emails.xlsx
+++ b/cohort_Emails.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mercy\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\practise\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9732"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -228,6 +228,18 @@
   </si>
   <si>
     <t>tashma19@gmail.com</t>
+  </si>
+  <si>
+    <t>tesijoanne@gmail.com</t>
+  </si>
+  <si>
+    <t>Kaweesimartinanderson@gmail.com</t>
+  </si>
+  <si>
+    <t>Joanne Mutesi</t>
+  </si>
+  <si>
+    <t>Martin Anderson Kaweesi</t>
   </si>
 </sst>
 </file>
@@ -570,20 +582,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.85546875" customWidth="1"/>
+    <col min="1" max="1" width="57.6640625" customWidth="1"/>
+    <col min="2" max="2" width="37.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -591,7 +603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -599,7 +611,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -607,7 +619,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -615,7 +627,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -623,7 +635,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -631,7 +643,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -639,7 +651,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -647,7 +659,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -655,7 +667,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -663,7 +675,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -671,7 +683,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -679,7 +691,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -687,7 +699,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -695,7 +707,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -703,196 +715,214 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B34">
+  <sortState ref="A2:B36">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B14" r:id="rId1"/>
-    <hyperlink ref="B17" r:id="rId2"/>
+    <hyperlink ref="B18" r:id="rId2"/>
     <hyperlink ref="B11" r:id="rId3"/>
-    <hyperlink ref="B25" r:id="rId4"/>
+    <hyperlink ref="B27" r:id="rId4"/>
     <hyperlink ref="B13" r:id="rId5"/>
     <hyperlink ref="B5" r:id="rId6"/>
-    <hyperlink ref="B21" r:id="rId7"/>
-    <hyperlink ref="B33" r:id="rId8"/>
+    <hyperlink ref="B23" r:id="rId7"/>
+    <hyperlink ref="B35" r:id="rId8"/>
     <hyperlink ref="B6" r:id="rId9"/>
-    <hyperlink ref="B34" r:id="rId10"/>
+    <hyperlink ref="B36" r:id="rId10"/>
     <hyperlink ref="B15" r:id="rId11"/>
-    <hyperlink ref="B28" r:id="rId12"/>
+    <hyperlink ref="B30" r:id="rId12"/>
     <hyperlink ref="B9" r:id="rId13"/>
-    <hyperlink ref="B18" r:id="rId14"/>
+    <hyperlink ref="B19" r:id="rId14"/>
     <hyperlink ref="B10" r:id="rId15"/>
-    <hyperlink ref="B32" r:id="rId16"/>
-    <hyperlink ref="B30" r:id="rId17"/>
+    <hyperlink ref="B34" r:id="rId16"/>
+    <hyperlink ref="B32" r:id="rId17"/>
     <hyperlink ref="B2" r:id="rId18"/>
-    <hyperlink ref="B27" r:id="rId19"/>
+    <hyperlink ref="B29" r:id="rId19"/>
     <hyperlink ref="B4" r:id="rId20"/>
-    <hyperlink ref="B26" r:id="rId21"/>
+    <hyperlink ref="B28" r:id="rId21"/>
     <hyperlink ref="B3" r:id="rId22"/>
     <hyperlink ref="B8" r:id="rId23"/>
-    <hyperlink ref="B29" r:id="rId24"/>
-    <hyperlink ref="B19" r:id="rId25"/>
-    <hyperlink ref="B20" r:id="rId26"/>
-    <hyperlink ref="B24" r:id="rId27"/>
+    <hyperlink ref="B31" r:id="rId24"/>
+    <hyperlink ref="B20" r:id="rId25"/>
+    <hyperlink ref="B22" r:id="rId26"/>
+    <hyperlink ref="B26" r:id="rId27"/>
     <hyperlink ref="B7" r:id="rId28"/>
-    <hyperlink ref="B22" r:id="rId29"/>
-    <hyperlink ref="B31" r:id="rId30"/>
-    <hyperlink ref="B16" r:id="rId31"/>
+    <hyperlink ref="B24" r:id="rId29"/>
+    <hyperlink ref="B33" r:id="rId30"/>
+    <hyperlink ref="B17" r:id="rId31"/>
     <hyperlink ref="B12" r:id="rId32"/>
-    <hyperlink ref="B23" r:id="rId33"/>
+    <hyperlink ref="B25" r:id="rId33"/>
+    <hyperlink ref="B16" r:id="rId34"/>
+    <hyperlink ref="B21" r:id="rId35"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>